<commit_message>
Joint Acc Creation LCY CAO - Sarib Shamim
</commit_message>
<xml_diff>
--- a/Excel Data/COAD_AccCreation.xlsx
+++ b/Excel Data/COAD_AccCreation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Cid</t>
   </si>
@@ -59,12 +59,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>9-00000000</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Jholder</t>
   </si>
   <si>
@@ -74,7 +68,37 @@
     <t>testing</t>
   </si>
   <si>
-    <t>TxnAttempts</t>
+    <t>ExpectedNumOfTxn</t>
+  </si>
+  <si>
+    <t>AC Screen list</t>
+  </si>
+  <si>
+    <t>8-02-200000</t>
+  </si>
+  <si>
+    <t>RelationCode</t>
+  </si>
+  <si>
+    <t>8-02</t>
+  </si>
+  <si>
+    <t>Below 1M</t>
+  </si>
+  <si>
+    <t>TurnoverM</t>
+  </si>
+  <si>
+    <t>TurnoverA</t>
+  </si>
+  <si>
+    <t>1M to 5M</t>
+  </si>
+  <si>
+    <t>debitTxnNum</t>
+  </si>
+  <si>
+    <t>TurnoverDebitMonth</t>
   </si>
 </sst>
 </file>
@@ -112,7 +136,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,16 +454,34 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>16</v>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001231</v>
       </c>
@@ -453,28 +495,46 @@
         <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>44931</v>
+        <v>20230106</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>16206304</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2">
         <v>20</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Joint Acc Creation FCY CAO - Sarib Shamim
</commit_message>
<xml_diff>
--- a/Excel Data/COAD_AccCreation.xlsx
+++ b/Excel Data/COAD_AccCreation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Cid</t>
   </si>
@@ -99,6 +100,21 @@
   </si>
   <si>
     <t>TurnoverDebitMonth</t>
+  </si>
+  <si>
+    <t>6-012</t>
+  </si>
+  <si>
+    <t>3-01</t>
+  </si>
+  <si>
+    <t>3-01-01</t>
+  </si>
+  <si>
+    <t>sbpSubSegment</t>
+  </si>
+  <si>
+    <t>3-01-01-0100</t>
   </si>
 </sst>
 </file>
@@ -419,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,4 +557,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11241908</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20230106</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>16206304</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Joint Acc Creation CAO scripts - Sarib Shamim
</commit_message>
<xml_diff>
--- a/Excel Data/COAD_AccCreation.xlsx
+++ b/Excel Data/COAD_AccCreation.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LCY current" sheetId="1" r:id="rId1"/>
+    <sheet name="LCY Saving" sheetId="2" r:id="rId2"/>
+    <sheet name="FCY current" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
   <si>
     <t>Cid</t>
   </si>
@@ -115,19 +116,49 @@
   </si>
   <si>
     <t>3-01-01-0100</t>
+  </si>
+  <si>
+    <t>1-003</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>20230107</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>3-14</t>
+  </si>
+  <si>
+    <t>3-14-030000</t>
+  </si>
+  <si>
+    <t>BioVersion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,9 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +468,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -690,4 +722,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>11699192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>16206304</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting 1 excel file - Sarib Shamim.
</commit_message>
<xml_diff>
--- a/Excel Data/COAD_AccCreation.xlsx
+++ b/Excel Data/COAD_AccCreation.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Workspace Functional Testing\Retail Ops\Excel Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcelliti5\IdeaProjects\Retail Project\Excel Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LCY current" sheetId="1" r:id="rId1"/>
     <sheet name="LCY Saving" sheetId="2" r:id="rId2"/>
     <sheet name="FCY current" sheetId="3" r:id="rId3"/>
-    <sheet name="FCY Saving" sheetId="4" r:id="rId4"/>
+    <sheet name="LCSavingAccountInputter" sheetId="4" r:id="rId4"/>
+    <sheet name="LCCurrentInputter" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
   <si>
     <t>Cid</t>
   </si>
@@ -143,13 +144,13 @@
     <t>BioVersion</t>
   </si>
   <si>
-    <t>6-003</t>
-  </si>
-  <si>
-    <t>hasan</t>
-  </si>
-  <si>
-    <t>aftab</t>
+    <t>Purpose of Bank Account</t>
+  </si>
+  <si>
+    <t>for property purpose use</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -739,7 +740,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="A1:XFD1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,136 +877,65 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>16806732</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>1007758835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1007414740</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
         <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2">
-        <v>16206304</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2">
-        <v>30</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-      <c r="P2">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2">
-        <v>30</v>
-      </c>
-      <c r="T2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>